<commit_message>
Mz and My added, using RHR conventions
</commit_message>
<xml_diff>
--- a/HourRegistration_A43.xlsx
+++ b/HourRegistration_A43.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmaio\Nextcloud\TU Delft\2019-2020\SVV\Do228-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174426C7-A872-4585-9E30-424A7A79CEEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B44B5C5F-0C12-4520-BC8E-B961E8952ED6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Project group</t>
   </si>
@@ -61,18 +67,6 @@
   </si>
   <si>
     <t>student id</t>
-  </si>
-  <si>
-    <t>id2</t>
-  </si>
-  <si>
-    <t>id3</t>
-  </si>
-  <si>
-    <t>id4</t>
-  </si>
-  <si>
-    <t>id5</t>
   </si>
   <si>
     <t>id6</t>
@@ -512,7 +506,7 @@
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D16" sqref="D16:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,13 +521,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -543,20 +537,20 @@
       <c r="D4" s="11">
         <v>4431138</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="11">
+        <v>4645669</v>
+      </c>
+      <c r="F4" s="11">
+        <v>4536908</v>
+      </c>
+      <c r="G4" s="11">
+        <v>4538420</v>
+      </c>
+      <c r="H4" s="11">
+        <v>4559118</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -602,10 +596,18 @@
       <c r="D8" s="5">
         <v>2</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
@@ -615,31 +617,57 @@
       <c r="D9" s="5">
         <v>4</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="E9" s="6">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6">
+        <v>4</v>
+      </c>
+      <c r="G9" s="6">
+        <v>4</v>
+      </c>
+      <c r="H9" s="6">
+        <v>4</v>
+      </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="D10" s="5">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6">
+        <v>4</v>
+      </c>
+      <c r="F10" s="6">
+        <v>6</v>
+      </c>
+      <c r="G10" s="6">
+        <v>4</v>
+      </c>
+      <c r="H10" s="6">
+        <v>8</v>
+      </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="D11" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="E11" s="9">
+        <v>5</v>
+      </c>
+      <c r="F11" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="G11" s="9">
+        <v>8.5</v>
+      </c>
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
     </row>
@@ -672,11 +700,15 @@
       <c r="C15" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5">
+        <v>6</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="6">
+        <v>4</v>
+      </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Cleaned directory for submission
</commit_message>
<xml_diff>
--- a/HourRegistration_A43.xlsx
+++ b/HourRegistration_A43.xlsx
@@ -5,33 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmaio\Nextcloud\TU Delft\2019-2020\SVV\Do228-Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmaio\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B44B5C5F-0C12-4520-BC8E-B961E8952ED6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFFD8EB-89B7-425F-8DAF-4D07332613D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4764" yWindow="1596" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Project group</t>
   </si>
@@ -67,9 +61,6 @@
   </si>
   <si>
     <t>student id</t>
-  </si>
-  <si>
-    <t>id6</t>
   </si>
   <si>
     <t>A43</t>
@@ -506,14 +497,14 @@
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D19"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
@@ -521,13 +512,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -549,8 +540,8 @@
       <c r="H4" s="11">
         <v>4559118</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>12</v>
+      <c r="I4" s="11">
+        <v>4672372</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -608,7 +599,9 @@
       <c r="H8" s="6">
         <v>0</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
@@ -629,7 +622,9 @@
       <c r="H9" s="6">
         <v>4</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
@@ -650,7 +645,9 @@
       <c r="H10" s="6">
         <v>8</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
@@ -668,8 +665,12 @@
       <c r="G11" s="9">
         <v>8.5</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="10"/>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -689,7 +690,9 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5">
+        <v>3</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -703,19 +706,29 @@
       <c r="D15" s="5">
         <v>6</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="E15" s="6">
+        <v>4</v>
+      </c>
+      <c r="F15" s="6">
+        <v>4</v>
+      </c>
+      <c r="G15" s="6">
+        <v>4</v>
+      </c>
       <c r="H15" s="6">
         <v>4</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5">
+        <v>4</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -726,31 +739,59 @@
       <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
+      <c r="D17" s="5">
+        <v>6</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4</v>
+      </c>
+      <c r="F17" s="6">
+        <v>6</v>
+      </c>
+      <c r="G17" s="6">
+        <v>4</v>
+      </c>
+      <c r="H17" s="6">
+        <v>4</v>
+      </c>
+      <c r="I17" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
+      <c r="D18" s="5">
+        <v>8</v>
+      </c>
+      <c r="E18" s="6">
+        <v>4</v>
+      </c>
+      <c r="F18" s="6">
+        <v>6</v>
+      </c>
+      <c r="G18" s="6">
+        <v>4</v>
+      </c>
+      <c r="H18" s="6">
+        <v>4</v>
+      </c>
+      <c r="I18" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="8">
+        <v>8</v>
+      </c>
       <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="F19" s="9">
+        <v>3</v>
+      </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
@@ -762,9 +803,13 @@
       <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>4</v>
+      </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3">
+        <v>4</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="4"/>
@@ -773,9 +818,13 @@
       <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="5">
+        <v>8</v>
+      </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="F22" s="6">
+        <v>6</v>
+      </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
@@ -784,56 +833,116 @@
       <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="7"/>
+      <c r="D23" s="5">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6">
+        <v>6</v>
+      </c>
+      <c r="F23" s="6">
+        <v>7</v>
+      </c>
+      <c r="G23" s="6">
+        <v>7</v>
+      </c>
+      <c r="H23" s="6">
+        <v>10</v>
+      </c>
+      <c r="I23" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="7"/>
+      <c r="D24" s="5">
+        <v>8</v>
+      </c>
+      <c r="E24" s="6">
+        <v>7</v>
+      </c>
+      <c r="F24" s="6">
+        <v>7</v>
+      </c>
+      <c r="G24" s="6">
+        <v>7</v>
+      </c>
+      <c r="H24" s="6">
+        <v>10</v>
+      </c>
+      <c r="I24" s="7">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="7"/>
+      <c r="D25" s="5">
+        <v>12</v>
+      </c>
+      <c r="E25" s="6">
+        <v>4</v>
+      </c>
+      <c r="F25" s="6">
+        <v>7</v>
+      </c>
+      <c r="G25" s="6">
+        <v>2</v>
+      </c>
+      <c r="H25" s="6">
+        <v>10</v>
+      </c>
+      <c r="I25" s="7">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="7"/>
+      <c r="D26" s="5">
+        <v>10</v>
+      </c>
+      <c r="E26" s="6">
+        <v>7</v>
+      </c>
+      <c r="F26" s="6">
+        <v>12</v>
+      </c>
+      <c r="G26" s="6">
+        <v>7</v>
+      </c>
+      <c r="H26" s="6">
+        <v>10</v>
+      </c>
+      <c r="I26" s="7">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="10"/>
+      <c r="D27" s="8">
+        <v>8</v>
+      </c>
+      <c r="E27" s="9">
+        <v>6</v>
+      </c>
+      <c r="F27" s="9">
+        <v>7</v>
+      </c>
+      <c r="G27" s="9">
+        <v>6</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>